<commit_message>
Add LsegWorkspace as a new data provider
Add LsegWorkspace as a new data provider implementation

- Implement `LsegWorkspace` class (`lseg_workspace.py`) with full support for market data,
  fundamental data, dividend data, split data, and currency data fetching via the
  Refinitiv/LSEG Workspace API
- Bulk fetching strategy with adaptive binary-split chunking for error resilience
- Fundamental data fetched in batches (max 30 fields/batch) to respect API field limits
- Dividend-adjusted price calculation integrated into the data processing pipeline
- Register LSEG-specific exceptions in `exceptions/__init__.py`
- Update `data_providers/__init__.py` and `configurator_interface.py` for LSEG integration
- Add `refinitiv-data` dependency in `pyproject.toml`

### Tests

Integration tests exist under `tests/integration/lseg_workspace/`
</commit_message>
<xml_diff>
--- a/templates/data_curator/Config/parameters_datacurator.xlsx
+++ b/templates/data_curator/Config/parameters_datacurator.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rinku\Current Projects\KaxaNuk\Open_FMP-Module\templates\data_curator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\data_curator\Data-Curator\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA755872-5E3E-49BF-9582-17CB12EA8B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,23 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
   <si>
     <t>parameter</t>
   </si>
@@ -275,9 +265,6 @@
     </r>
   </si>
   <si>
-    <t>financial_modeling_prep</t>
-  </si>
-  <si>
     <t>info</t>
   </si>
   <si>
@@ -783,15 +770,21 @@
   <si>
     <t>c_simple_moving_average_252d_close_split_adjusted</t>
   </si>
+  <si>
+    <t>AAPL.OQ</t>
+  </si>
+  <si>
+    <t>lseg_workspace</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -860,13 +853,11 @@
       <sz val="10"/>
       <color rgb="FF00B0F0"/>
       <name val="Montserrat"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0070C0"/>
       <name val="Montserrat"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1034,8 +1025,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -1385,25 +1376,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.25" style="6" customWidth="1"/>
-    <col min="3" max="3" width="79.625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="33.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="79.54296875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1414,51 +1405,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>66</v>
+        <v>230</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="25.5">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>66</v>
+        <v>230</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="25.5">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="16">
-        <v>32874</v>
+        <v>43832</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="25.5">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="16">
-        <v>45657</v>
+        <v>46066</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
@@ -1469,7 +1460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
@@ -1480,34 +1471,34 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="25.5">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="15"/>
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:3" ht="25.5">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="25.5">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.35">
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1515,22 +1506,22 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"financial_modeling_prep,yahoo_finance"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"financial_modeling_prep,yahoo_finance,lseg_workspace"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>"financial_modeling_prep,none"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"financial_modeling_prep,lseg_workspace,none"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>B4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"debug,info,warning,error,critical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"quarterly,annual"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"csv,parquet"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1540,29 +1531,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="74.625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="9.125" style="4"/>
+    <col min="1" max="1" width="19.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="74.54296875" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>70</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -1571,24 +1567,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A205" sqref="A205"/>
+      <selection pane="bottomRight" activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="73.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="91.875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="9.125" style="4"/>
+    <col min="1" max="1" width="73.453125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="91.81640625" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -1596,1022 +1592,1022 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="18"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="18"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="18"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="18"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="18"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="18"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="18"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="18"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="18"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" s="21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="21" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="23" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="23" t="s">
+      <c r="B27" s="20"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="20"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="23" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="23" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A33" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="23" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34" s="23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="23" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A35" s="23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="23" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A36" s="23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="23" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A37" s="23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="23" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A38" s="23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="23" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A39" s="23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="23" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A40" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="23" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A41" s="23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A42" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A43" s="23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A44" s="23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A45" s="23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="23" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A46" s="23" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="23" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A47" s="23" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A48" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A49" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A50" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="23" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A51" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="23" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A52" s="23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="23" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A53" s="23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="23" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A54" s="23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="23" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A55" s="23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="23" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A56" s="23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="23" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A57" s="23" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="23" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A58" s="23" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="23" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A59" s="23" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A60" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A61" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A62" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A63" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A64" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A65" s="23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="23" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A66" s="23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="23" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A67" s="23" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="23" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A68" s="23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="23" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A69" s="23" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="23" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A70" s="23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A71" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A72" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A73" s="23" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="23" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A74" s="23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="23" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A75" s="23" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="23" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A76" s="23" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="23" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A77" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="23" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A78" s="23" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="23" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A79" s="23" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="23" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A80" s="24" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="24" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A81" s="24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A82" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A83" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A84" s="24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="24" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A85" s="24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="24" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A86" s="24" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="24" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A87" s="24" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A88" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A89" s="24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A90" s="24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A91" s="24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A92" s="24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A93" s="24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="24" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A94" s="24" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="24" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A95" s="24" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="24" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A96" s="24" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="24" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A97" s="24" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="24" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A98" s="24" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="24" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A99" s="24" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
-      <c r="A99" s="24" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A100" s="24" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="24" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A101" s="24" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
-      <c r="A101" s="24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A102" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A103" s="24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A104" s="24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104" s="24" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A105" s="24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="24" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A106" s="24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
-      <c r="A106" s="24" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A107" s="24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
-      <c r="A107" s="24" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A108" s="24" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="24" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A109" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
-      <c r="A109" s="24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A110" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A111" s="24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A112" s="24" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
-      <c r="A112" s="24" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A113" s="24" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
-      <c r="A113" s="24" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A114" s="24" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
-      <c r="A114" s="24" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A115" s="24" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
-      <c r="A115" s="24" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A116" s="24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A117" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A118" s="25" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
-      <c r="A118" s="25" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A119" s="25" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
-      <c r="A119" s="25" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A120" s="25" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
-      <c r="A120" s="25" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A121" s="25" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
-      <c r="A121" s="25" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A122" s="25" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
-      <c r="A122" s="25" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A123" s="25" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
-      <c r="A123" s="25" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A124" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
-      <c r="A124" s="25" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A125" s="25" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
-      <c r="A125" s="25" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A126" s="25" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
-      <c r="A126" s="25" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A127" s="25" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
-      <c r="A127" s="25" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A128" s="25" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
-      <c r="A128" s="25" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A129" s="25" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
-      <c r="A129" s="25" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A130" s="25" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
-      <c r="A130" s="25" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A131" s="25" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
-      <c r="A131" s="25" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A132" s="25" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
-      <c r="A132" s="25" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A133" s="25" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
-      <c r="A133" s="25" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A134" s="25" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
-      <c r="A134" s="25" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A135" s="25" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
-      <c r="A135" s="25" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A136" s="25" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
-      <c r="A136" s="25" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A137" s="25" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
-      <c r="A137" s="25" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A138" s="25" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
-      <c r="A138" s="25" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A139" s="25" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
-      <c r="A139" s="25" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A140" s="25" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
-      <c r="A140" s="25" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A141" s="25" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
-      <c r="A141" s="25" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A142" s="25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
-      <c r="A142" s="25" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A143" s="25" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
-      <c r="A143" s="25" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A144" s="25" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
-      <c r="A144" s="25" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A145" s="25" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
-      <c r="A145" s="25" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A146" s="25" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
-      <c r="A146" s="25" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A147" s="25" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
-      <c r="A147" s="25" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A148" s="25" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
-      <c r="A148" s="25" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A149" s="27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A150" s="27" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A151" s="27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A152" s="27" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A153" s="27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A154" s="27" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A155" s="27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A156" s="27" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A157" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A158" s="26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A159" s="22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A160" s="22" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
-      <c r="A160" s="22" t="s">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A161" s="22" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
-      <c r="A161" s="22" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A162" s="22" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
-      <c r="A162" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A163" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A164" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A165" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A166" s="22" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
-      <c r="A166" s="22" t="s">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A167" s="22" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
-      <c r="A167" s="22" t="s">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A168" s="22" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
-      <c r="A168" s="22" t="s">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A169" s="22" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
-      <c r="A169" s="22" t="s">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A170" s="22" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
-      <c r="A170" s="22" t="s">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A171" s="22" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
-      <c r="A171" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A172" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A173" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A174" s="22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A175" s="22" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
-      <c r="A175" s="22" t="s">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A176" s="22" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
-      <c r="A176" s="22" t="s">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A177" s="22" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
-      <c r="A177" s="22" t="s">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A178" s="22" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
-      <c r="A178" s="22" t="s">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A179" s="22" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
-      <c r="A179" s="22" t="s">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A180" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
-      <c r="A180" s="22" t="s">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A181" s="22" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
-      <c r="A181" s="22" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A182" s="22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A183" s="22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A184" s="22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A185" s="22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A186" s="22" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
-      <c r="A186" s="22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A187" s="22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A188" s="22" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A189" s="22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
-      <c r="A189" s="22" t="s">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A190" s="22" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
-      <c r="A190" s="22" t="s">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A191" s="22" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
-      <c r="A191" s="22" t="s">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A192" s="22" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
-      <c r="A192" s="22" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A193" s="22" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
-      <c r="A193" s="22" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A194" s="22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A195" s="22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A196" s="22" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
-      <c r="A196" s="22" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A197" s="22" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
-      <c r="A197" s="22" t="s">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A198" s="22" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
-      <c r="A198" s="22" t="s">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A199" s="22" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="199" spans="1:2">
-      <c r="A199" s="22" t="s">
+      <c r="B199" s="20"/>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A200" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="B199" s="20"/>
-    </row>
-    <row r="200" spans="1:2">
-      <c r="A200" s="22" t="s">
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A201" s="22" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
-      <c r="A201" s="22" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A202" s="22" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
-      <c r="A202" s="22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A205" s="20"/>
     </row>
   </sheetData>

</xml_diff>